<commit_message>
Update Medical Al Disease Diagnostic Tool.Gantt.Chart.xlsx
</commit_message>
<xml_diff>
--- a/Medical Al Disease Diagnostic Tool.Gantt.Chart.xlsx
+++ b/Medical Al Disease Diagnostic Tool.Gantt.Chart.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804D345E-57A4-4F31-85E8-8B5CD48FE366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4EF566-B53D-486E-B875-F0A3C08FE0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31770" yWindow="0" windowWidth="21075" windowHeight="15600" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="420" windowWidth="21075" windowHeight="15600" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -202,9 +202,6 @@
     <t>Project Snapshot 2</t>
   </si>
   <si>
-    <t>Create Readme files, gantt charts, Git wiki,Project artifacts</t>
-  </si>
-  <si>
     <t>Project Snapshot 3</t>
   </si>
   <si>
@@ -215,6 +212,18 @@
   </si>
   <si>
     <t>M. Haidari  K. Westbrook, Kelvin luk</t>
+  </si>
+  <si>
+    <t>Mansoor</t>
+  </si>
+  <si>
+    <t>READme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System Document Diesgn </t>
+  </si>
+  <si>
+    <t>Gantt chart Phase 1, Git Wiki</t>
   </si>
 </sst>
 </file>
@@ -892,6 +901,13 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -904,13 +920,6 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1480,8 +1489,8 @@
   <dimension ref="A1:BL38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1501,7 +1510,7 @@
     <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="59"/>
       <c r="B1" s="79" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1524,343 +1533,343 @@
         <v>29</v>
       </c>
       <c r="B3" s="77" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="89" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="90"/>
-      <c r="E3" s="88">
+      <c r="D3" s="86"/>
+      <c r="E3" s="91">
         <f ca="1">TODAY()</f>
-        <v>44974</v>
-      </c>
-      <c r="F3" s="88"/>
+        <v>44977</v>
+      </c>
+      <c r="F3" s="91"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="89" t="s">
+      <c r="C4" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="90"/>
+      <c r="D4" s="86"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="85">
+      <c r="I4" s="88">
         <f ca="1">I5</f>
-        <v>44970</v>
-      </c>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="87"/>
-      <c r="P4" s="85">
+        <v>44977</v>
+      </c>
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="89"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="88">
         <f ca="1">P5</f>
-        <v>44977</v>
-      </c>
-      <c r="Q4" s="86"/>
-      <c r="R4" s="86"/>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="86"/>
-      <c r="V4" s="87"/>
-      <c r="W4" s="85">
+        <v>44984</v>
+      </c>
+      <c r="Q4" s="89"/>
+      <c r="R4" s="89"/>
+      <c r="S4" s="89"/>
+      <c r="T4" s="89"/>
+      <c r="U4" s="89"/>
+      <c r="V4" s="90"/>
+      <c r="W4" s="88">
         <f ca="1">W5</f>
-        <v>44984</v>
-      </c>
-      <c r="X4" s="86"/>
-      <c r="Y4" s="86"/>
-      <c r="Z4" s="86"/>
-      <c r="AA4" s="86"/>
-      <c r="AB4" s="86"/>
-      <c r="AC4" s="87"/>
-      <c r="AD4" s="85">
+        <v>44991</v>
+      </c>
+      <c r="X4" s="89"/>
+      <c r="Y4" s="89"/>
+      <c r="Z4" s="89"/>
+      <c r="AA4" s="89"/>
+      <c r="AB4" s="89"/>
+      <c r="AC4" s="90"/>
+      <c r="AD4" s="88">
         <f ca="1">AD5</f>
-        <v>44991</v>
-      </c>
-      <c r="AE4" s="86"/>
-      <c r="AF4" s="86"/>
-      <c r="AG4" s="86"/>
-      <c r="AH4" s="86"/>
-      <c r="AI4" s="86"/>
-      <c r="AJ4" s="87"/>
-      <c r="AK4" s="85">
+        <v>44998</v>
+      </c>
+      <c r="AE4" s="89"/>
+      <c r="AF4" s="89"/>
+      <c r="AG4" s="89"/>
+      <c r="AH4" s="89"/>
+      <c r="AI4" s="89"/>
+      <c r="AJ4" s="90"/>
+      <c r="AK4" s="88">
         <f ca="1">AK5</f>
-        <v>44998</v>
-      </c>
-      <c r="AL4" s="86"/>
-      <c r="AM4" s="86"/>
-      <c r="AN4" s="86"/>
-      <c r="AO4" s="86"/>
-      <c r="AP4" s="86"/>
-      <c r="AQ4" s="87"/>
-      <c r="AR4" s="85">
+        <v>45005</v>
+      </c>
+      <c r="AL4" s="89"/>
+      <c r="AM4" s="89"/>
+      <c r="AN4" s="89"/>
+      <c r="AO4" s="89"/>
+      <c r="AP4" s="89"/>
+      <c r="AQ4" s="90"/>
+      <c r="AR4" s="88">
         <f ca="1">AR5</f>
-        <v>45005</v>
-      </c>
-      <c r="AS4" s="86"/>
-      <c r="AT4" s="86"/>
-      <c r="AU4" s="86"/>
-      <c r="AV4" s="86"/>
-      <c r="AW4" s="86"/>
-      <c r="AX4" s="87"/>
-      <c r="AY4" s="85">
+        <v>45012</v>
+      </c>
+      <c r="AS4" s="89"/>
+      <c r="AT4" s="89"/>
+      <c r="AU4" s="89"/>
+      <c r="AV4" s="89"/>
+      <c r="AW4" s="89"/>
+      <c r="AX4" s="90"/>
+      <c r="AY4" s="88">
         <f ca="1">AY5</f>
-        <v>45012</v>
-      </c>
-      <c r="AZ4" s="86"/>
-      <c r="BA4" s="86"/>
-      <c r="BB4" s="86"/>
-      <c r="BC4" s="86"/>
-      <c r="BD4" s="86"/>
-      <c r="BE4" s="87"/>
-      <c r="BF4" s="85">
+        <v>45019</v>
+      </c>
+      <c r="AZ4" s="89"/>
+      <c r="BA4" s="89"/>
+      <c r="BB4" s="89"/>
+      <c r="BC4" s="89"/>
+      <c r="BD4" s="89"/>
+      <c r="BE4" s="90"/>
+      <c r="BF4" s="88">
         <f ca="1">BF5</f>
-        <v>45019</v>
-      </c>
-      <c r="BG4" s="86"/>
-      <c r="BH4" s="86"/>
-      <c r="BI4" s="86"/>
-      <c r="BJ4" s="86"/>
-      <c r="BK4" s="86"/>
-      <c r="BL4" s="87"/>
+        <v>45026</v>
+      </c>
+      <c r="BG4" s="89"/>
+      <c r="BH4" s="89"/>
+      <c r="BI4" s="89"/>
+      <c r="BJ4" s="89"/>
+      <c r="BK4" s="89"/>
+      <c r="BL4" s="90"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="91"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
       <c r="I5" s="11">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>44970</v>
+        <v>44977</v>
       </c>
       <c r="J5" s="10">
         <f ca="1">I5+1</f>
-        <v>44971</v>
+        <v>44978</v>
       </c>
       <c r="K5" s="10">
         <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
-        <v>44972</v>
+        <v>44979</v>
       </c>
       <c r="L5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44973</v>
+        <v>44980</v>
       </c>
       <c r="M5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44974</v>
+        <v>44981</v>
       </c>
       <c r="N5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44975</v>
+        <v>44982</v>
       </c>
       <c r="O5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44976</v>
+        <v>44983</v>
       </c>
       <c r="P5" s="11">
         <f ca="1">O5+1</f>
-        <v>44977</v>
+        <v>44984</v>
       </c>
       <c r="Q5" s="10">
         <f ca="1">P5+1</f>
-        <v>44978</v>
+        <v>44985</v>
       </c>
       <c r="R5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44979</v>
+        <v>44986</v>
       </c>
       <c r="S5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44980</v>
+        <v>44987</v>
       </c>
       <c r="T5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44981</v>
+        <v>44988</v>
       </c>
       <c r="U5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44982</v>
+        <v>44989</v>
       </c>
       <c r="V5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44983</v>
+        <v>44990</v>
       </c>
       <c r="W5" s="11">
         <f ca="1">V5+1</f>
-        <v>44984</v>
+        <v>44991</v>
       </c>
       <c r="X5" s="10">
         <f ca="1">W5+1</f>
-        <v>44985</v>
+        <v>44992</v>
       </c>
       <c r="Y5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44986</v>
+        <v>44993</v>
       </c>
       <c r="Z5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44987</v>
+        <v>44994</v>
       </c>
       <c r="AA5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44988</v>
+        <v>44995</v>
       </c>
       <c r="AB5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44989</v>
+        <v>44996</v>
       </c>
       <c r="AC5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44990</v>
+        <v>44997</v>
       </c>
       <c r="AD5" s="11">
         <f ca="1">AC5+1</f>
-        <v>44991</v>
+        <v>44998</v>
       </c>
       <c r="AE5" s="10">
         <f ca="1">AD5+1</f>
-        <v>44992</v>
+        <v>44999</v>
       </c>
       <c r="AF5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44993</v>
+        <v>45000</v>
       </c>
       <c r="AG5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44994</v>
+        <v>45001</v>
       </c>
       <c r="AH5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44995</v>
+        <v>45002</v>
       </c>
       <c r="AI5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44996</v>
+        <v>45003</v>
       </c>
       <c r="AJ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44997</v>
+        <v>45004</v>
       </c>
       <c r="AK5" s="11">
         <f ca="1">AJ5+1</f>
-        <v>44998</v>
+        <v>45005</v>
       </c>
       <c r="AL5" s="10">
         <f ca="1">AK5+1</f>
-        <v>44999</v>
+        <v>45006</v>
       </c>
       <c r="AM5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45000</v>
+        <v>45007</v>
       </c>
       <c r="AN5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45001</v>
+        <v>45008</v>
       </c>
       <c r="AO5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45002</v>
+        <v>45009</v>
       </c>
       <c r="AP5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45003</v>
+        <v>45010</v>
       </c>
       <c r="AQ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45004</v>
+        <v>45011</v>
       </c>
       <c r="AR5" s="11">
         <f ca="1">AQ5+1</f>
-        <v>45005</v>
+        <v>45012</v>
       </c>
       <c r="AS5" s="10">
         <f ca="1">AR5+1</f>
-        <v>45006</v>
+        <v>45013</v>
       </c>
       <c r="AT5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45007</v>
+        <v>45014</v>
       </c>
       <c r="AU5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45008</v>
+        <v>45015</v>
       </c>
       <c r="AV5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45009</v>
+        <v>45016</v>
       </c>
       <c r="AW5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45010</v>
+        <v>45017</v>
       </c>
       <c r="AX5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45011</v>
+        <v>45018</v>
       </c>
       <c r="AY5" s="11">
         <f ca="1">AX5+1</f>
-        <v>45012</v>
+        <v>45019</v>
       </c>
       <c r="AZ5" s="10">
         <f ca="1">AY5+1</f>
-        <v>45013</v>
+        <v>45020</v>
       </c>
       <c r="BA5" s="10">
         <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
-        <v>45014</v>
+        <v>45021</v>
       </c>
       <c r="BB5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45015</v>
+        <v>45022</v>
       </c>
       <c r="BC5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45016</v>
+        <v>45023</v>
       </c>
       <c r="BD5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45017</v>
+        <v>45024</v>
       </c>
       <c r="BE5" s="12">
         <f t="shared" ca="1" si="1"/>
-        <v>45018</v>
+        <v>45025</v>
       </c>
       <c r="BF5" s="11">
         <f ca="1">BE5+1</f>
-        <v>45019</v>
+        <v>45026</v>
       </c>
       <c r="BG5" s="10">
         <f ca="1">BF5+1</f>
-        <v>45020</v>
+        <v>45027</v>
       </c>
       <c r="BH5" s="10">
         <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>45021</v>
+        <v>45028</v>
       </c>
       <c r="BI5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>45022</v>
+        <v>45029</v>
       </c>
       <c r="BJ5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>45023</v>
+        <v>45030</v>
       </c>
       <c r="BK5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>45024</v>
+        <v>45031</v>
       </c>
       <c r="BL5" s="12">
         <f t="shared" ca="1" si="2"/>
-        <v>45025</v>
+        <v>45032</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2256,24 +2265,24 @@
         <v>34</v>
       </c>
       <c r="B9" s="80" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C9" s="69" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D9" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="63">
-        <v>44616</v>
+        <v>44602</v>
       </c>
       <c r="F9" s="63">
-        <v>44619</v>
+        <v>44612</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="17">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="I9" s="44"/>
       <c r="J9" s="44"/>
@@ -2334,13 +2343,17 @@
     </row>
     <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="59"/>
-      <c r="B10" s="80"/>
-      <c r="C10" s="69"/>
+      <c r="B10" s="80" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="69" t="s">
+        <v>46</v>
+      </c>
       <c r="D10" s="22">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E10" s="63">
-        <v>44612</v>
+        <v>44602</v>
       </c>
       <c r="F10" s="63">
         <v>44616</v>
@@ -2406,13 +2419,17 @@
     </row>
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="59"/>
-      <c r="B11" s="80"/>
-      <c r="C11" s="69"/>
+      <c r="B11" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="69" t="s">
+        <v>46</v>
+      </c>
       <c r="D11" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="63">
-        <v>44617</v>
+        <v>44602</v>
       </c>
       <c r="F11" s="63">
         <v>44618</v>
@@ -2992,7 +3009,7 @@
         <v>25</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" s="71"/>
       <c r="D19" s="29"/>
@@ -3934,7 +3951,7 @@
     <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="58"/>
       <c r="B32" s="84" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C32" s="74" t="s">
         <v>38</v>
@@ -4243,11 +4260,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4255,6 +4267,11 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
   <conditionalFormatting sqref="D7:D35">

</xml_diff>

<commit_message>
added License in READ ME.
</commit_message>
<xml_diff>
--- a/Medical Al Disease Diagnostic Tool.Gantt.Chart.xlsx
+++ b/Medical Al Disease Diagnostic Tool.Gantt.Chart.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4EF566-B53D-486E-B875-F0A3C08FE0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1115494-6120-47C6-A188-C298C638C107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="420" windowWidth="21075" windowHeight="15600" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1710" yWindow="1860" windowWidth="25380" windowHeight="11385" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>Gantt chart Phase 1, Git Wiki</t>
+  </si>
+  <si>
+    <t>Mansoor, Kelvin</t>
   </si>
 </sst>
 </file>
@@ -901,6 +904,18 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -908,18 +923,6 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1490,7 +1493,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X10" sqref="X10"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1535,118 +1538,118 @@
       <c r="B3" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="85" t="s">
+      <c r="C3" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="86"/>
-      <c r="E3" s="91">
+      <c r="D3" s="90"/>
+      <c r="E3" s="88">
         <f ca="1">TODAY()</f>
         <v>44977</v>
       </c>
-      <c r="F3" s="91"/>
+      <c r="F3" s="88"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="85" t="s">
+      <c r="C4" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="86"/>
+      <c r="D4" s="90"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="88">
+      <c r="I4" s="85">
         <f ca="1">I5</f>
         <v>44977</v>
       </c>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="90"/>
-      <c r="P4" s="88">
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="85">
         <f ca="1">P5</f>
         <v>44984</v>
       </c>
-      <c r="Q4" s="89"/>
-      <c r="R4" s="89"/>
-      <c r="S4" s="89"/>
-      <c r="T4" s="89"/>
-      <c r="U4" s="89"/>
-      <c r="V4" s="90"/>
-      <c r="W4" s="88">
+      <c r="Q4" s="86"/>
+      <c r="R4" s="86"/>
+      <c r="S4" s="86"/>
+      <c r="T4" s="86"/>
+      <c r="U4" s="86"/>
+      <c r="V4" s="87"/>
+      <c r="W4" s="85">
         <f ca="1">W5</f>
         <v>44991</v>
       </c>
-      <c r="X4" s="89"/>
-      <c r="Y4" s="89"/>
-      <c r="Z4" s="89"/>
-      <c r="AA4" s="89"/>
-      <c r="AB4" s="89"/>
-      <c r="AC4" s="90"/>
-      <c r="AD4" s="88">
+      <c r="X4" s="86"/>
+      <c r="Y4" s="86"/>
+      <c r="Z4" s="86"/>
+      <c r="AA4" s="86"/>
+      <c r="AB4" s="86"/>
+      <c r="AC4" s="87"/>
+      <c r="AD4" s="85">
         <f ca="1">AD5</f>
         <v>44998</v>
       </c>
-      <c r="AE4" s="89"/>
-      <c r="AF4" s="89"/>
-      <c r="AG4" s="89"/>
-      <c r="AH4" s="89"/>
-      <c r="AI4" s="89"/>
-      <c r="AJ4" s="90"/>
-      <c r="AK4" s="88">
+      <c r="AE4" s="86"/>
+      <c r="AF4" s="86"/>
+      <c r="AG4" s="86"/>
+      <c r="AH4" s="86"/>
+      <c r="AI4" s="86"/>
+      <c r="AJ4" s="87"/>
+      <c r="AK4" s="85">
         <f ca="1">AK5</f>
         <v>45005</v>
       </c>
-      <c r="AL4" s="89"/>
-      <c r="AM4" s="89"/>
-      <c r="AN4" s="89"/>
-      <c r="AO4" s="89"/>
-      <c r="AP4" s="89"/>
-      <c r="AQ4" s="90"/>
-      <c r="AR4" s="88">
+      <c r="AL4" s="86"/>
+      <c r="AM4" s="86"/>
+      <c r="AN4" s="86"/>
+      <c r="AO4" s="86"/>
+      <c r="AP4" s="86"/>
+      <c r="AQ4" s="87"/>
+      <c r="AR4" s="85">
         <f ca="1">AR5</f>
         <v>45012</v>
       </c>
-      <c r="AS4" s="89"/>
-      <c r="AT4" s="89"/>
-      <c r="AU4" s="89"/>
-      <c r="AV4" s="89"/>
-      <c r="AW4" s="89"/>
-      <c r="AX4" s="90"/>
-      <c r="AY4" s="88">
+      <c r="AS4" s="86"/>
+      <c r="AT4" s="86"/>
+      <c r="AU4" s="86"/>
+      <c r="AV4" s="86"/>
+      <c r="AW4" s="86"/>
+      <c r="AX4" s="87"/>
+      <c r="AY4" s="85">
         <f ca="1">AY5</f>
         <v>45019</v>
       </c>
-      <c r="AZ4" s="89"/>
-      <c r="BA4" s="89"/>
-      <c r="BB4" s="89"/>
-      <c r="BC4" s="89"/>
-      <c r="BD4" s="89"/>
-      <c r="BE4" s="90"/>
-      <c r="BF4" s="88">
+      <c r="AZ4" s="86"/>
+      <c r="BA4" s="86"/>
+      <c r="BB4" s="86"/>
+      <c r="BC4" s="86"/>
+      <c r="BD4" s="86"/>
+      <c r="BE4" s="87"/>
+      <c r="BF4" s="85">
         <f ca="1">BF5</f>
         <v>45026</v>
       </c>
-      <c r="BG4" s="89"/>
-      <c r="BH4" s="89"/>
-      <c r="BI4" s="89"/>
-      <c r="BJ4" s="89"/>
-      <c r="BK4" s="89"/>
-      <c r="BL4" s="90"/>
+      <c r="BG4" s="86"/>
+      <c r="BH4" s="86"/>
+      <c r="BI4" s="86"/>
+      <c r="BJ4" s="86"/>
+      <c r="BK4" s="86"/>
+      <c r="BL4" s="87"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
       <c r="I5" s="11">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44977</v>
@@ -2268,7 +2271,7 @@
         <v>48</v>
       </c>
       <c r="C9" s="69" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D9" s="22">
         <v>1</v>
@@ -2423,7 +2426,7 @@
         <v>47</v>
       </c>
       <c r="C11" s="69" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D11" s="22">
         <v>1</v>
@@ -4260,6 +4263,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4267,11 +4275,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
   <conditionalFormatting sqref="D7:D35">

</xml_diff>

<commit_message>
added the first pycharm into git repo
</commit_message>
<xml_diff>
--- a/Medical Al Disease Diagnostic Tool.Gantt.Chart.xlsx
+++ b/Medical Al Disease Diagnostic Tool.Gantt.Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1115494-6120-47C6-A188-C298C638C107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C570BE7-D6EE-4625-B677-C50A24E628FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1710" yWindow="1860" windowWidth="25380" windowHeight="11385" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1493,7 +1493,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
File Io  / read excel data
</commit_message>
<xml_diff>
--- a/Medical Al Disease Diagnostic Tool.Gantt.Chart.xlsx
+++ b/Medical Al Disease Diagnostic Tool.Gantt.Chart.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C570BE7-D6EE-4625-B677-C50A24E628FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DCCCA8-BCF4-4019-B0E6-A37FE6B7A0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="1860" windowWidth="25380" windowHeight="11385" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1815" yWindow="2805" windowWidth="25380" windowHeight="11385" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -227,6 +227,12 @@
   </si>
   <si>
     <t>Mansoor, Kelvin</t>
+  </si>
+  <si>
+    <t>Kelvin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File IO. Reading xlse data, and Display data </t>
   </si>
 </sst>
 </file>
@@ -1493,7 +1499,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1544,7 +1550,7 @@
       <c r="D3" s="90"/>
       <c r="E3" s="88">
         <f ca="1">TODAY()</f>
-        <v>44977</v>
+        <v>44990</v>
       </c>
       <c r="F3" s="88"/>
     </row>
@@ -1561,7 +1567,7 @@
       </c>
       <c r="I4" s="85">
         <f ca="1">I5</f>
-        <v>44977</v>
+        <v>44991</v>
       </c>
       <c r="J4" s="86"/>
       <c r="K4" s="86"/>
@@ -1571,7 +1577,7 @@
       <c r="O4" s="87"/>
       <c r="P4" s="85">
         <f ca="1">P5</f>
-        <v>44984</v>
+        <v>44998</v>
       </c>
       <c r="Q4" s="86"/>
       <c r="R4" s="86"/>
@@ -1581,7 +1587,7 @@
       <c r="V4" s="87"/>
       <c r="W4" s="85">
         <f ca="1">W5</f>
-        <v>44991</v>
+        <v>45005</v>
       </c>
       <c r="X4" s="86"/>
       <c r="Y4" s="86"/>
@@ -1591,7 +1597,7 @@
       <c r="AC4" s="87"/>
       <c r="AD4" s="85">
         <f ca="1">AD5</f>
-        <v>44998</v>
+        <v>45012</v>
       </c>
       <c r="AE4" s="86"/>
       <c r="AF4" s="86"/>
@@ -1601,7 +1607,7 @@
       <c r="AJ4" s="87"/>
       <c r="AK4" s="85">
         <f ca="1">AK5</f>
-        <v>45005</v>
+        <v>45019</v>
       </c>
       <c r="AL4" s="86"/>
       <c r="AM4" s="86"/>
@@ -1611,7 +1617,7 @@
       <c r="AQ4" s="87"/>
       <c r="AR4" s="85">
         <f ca="1">AR5</f>
-        <v>45012</v>
+        <v>45026</v>
       </c>
       <c r="AS4" s="86"/>
       <c r="AT4" s="86"/>
@@ -1621,7 +1627,7 @@
       <c r="AX4" s="87"/>
       <c r="AY4" s="85">
         <f ca="1">AY5</f>
-        <v>45019</v>
+        <v>45033</v>
       </c>
       <c r="AZ4" s="86"/>
       <c r="BA4" s="86"/>
@@ -1631,7 +1637,7 @@
       <c r="BE4" s="87"/>
       <c r="BF4" s="85">
         <f ca="1">BF5</f>
-        <v>45026</v>
+        <v>45040</v>
       </c>
       <c r="BG4" s="86"/>
       <c r="BH4" s="86"/>
@@ -1652,227 +1658,227 @@
       <c r="G5" s="91"/>
       <c r="I5" s="11">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>44977</v>
+        <v>44991</v>
       </c>
       <c r="J5" s="10">
         <f ca="1">I5+1</f>
-        <v>44978</v>
+        <v>44992</v>
       </c>
       <c r="K5" s="10">
         <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
-        <v>44979</v>
+        <v>44993</v>
       </c>
       <c r="L5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44980</v>
+        <v>44994</v>
       </c>
       <c r="M5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44981</v>
+        <v>44995</v>
       </c>
       <c r="N5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44982</v>
+        <v>44996</v>
       </c>
       <c r="O5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44983</v>
+        <v>44997</v>
       </c>
       <c r="P5" s="11">
         <f ca="1">O5+1</f>
-        <v>44984</v>
+        <v>44998</v>
       </c>
       <c r="Q5" s="10">
         <f ca="1">P5+1</f>
-        <v>44985</v>
+        <v>44999</v>
       </c>
       <c r="R5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44986</v>
+        <v>45000</v>
       </c>
       <c r="S5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44987</v>
+        <v>45001</v>
       </c>
       <c r="T5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44988</v>
+        <v>45002</v>
       </c>
       <c r="U5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44989</v>
+        <v>45003</v>
       </c>
       <c r="V5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44990</v>
+        <v>45004</v>
       </c>
       <c r="W5" s="11">
         <f ca="1">V5+1</f>
-        <v>44991</v>
+        <v>45005</v>
       </c>
       <c r="X5" s="10">
         <f ca="1">W5+1</f>
-        <v>44992</v>
+        <v>45006</v>
       </c>
       <c r="Y5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44993</v>
+        <v>45007</v>
       </c>
       <c r="Z5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44994</v>
+        <v>45008</v>
       </c>
       <c r="AA5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44995</v>
+        <v>45009</v>
       </c>
       <c r="AB5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44996</v>
+        <v>45010</v>
       </c>
       <c r="AC5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44997</v>
+        <v>45011</v>
       </c>
       <c r="AD5" s="11">
         <f ca="1">AC5+1</f>
-        <v>44998</v>
+        <v>45012</v>
       </c>
       <c r="AE5" s="10">
         <f ca="1">AD5+1</f>
-        <v>44999</v>
+        <v>45013</v>
       </c>
       <c r="AF5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45000</v>
+        <v>45014</v>
       </c>
       <c r="AG5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45001</v>
+        <v>45015</v>
       </c>
       <c r="AH5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45002</v>
+        <v>45016</v>
       </c>
       <c r="AI5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45003</v>
+        <v>45017</v>
       </c>
       <c r="AJ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45004</v>
+        <v>45018</v>
       </c>
       <c r="AK5" s="11">
         <f ca="1">AJ5+1</f>
-        <v>45005</v>
+        <v>45019</v>
       </c>
       <c r="AL5" s="10">
         <f ca="1">AK5+1</f>
-        <v>45006</v>
+        <v>45020</v>
       </c>
       <c r="AM5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45007</v>
+        <v>45021</v>
       </c>
       <c r="AN5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45008</v>
+        <v>45022</v>
       </c>
       <c r="AO5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45009</v>
+        <v>45023</v>
       </c>
       <c r="AP5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45010</v>
+        <v>45024</v>
       </c>
       <c r="AQ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45011</v>
+        <v>45025</v>
       </c>
       <c r="AR5" s="11">
         <f ca="1">AQ5+1</f>
-        <v>45012</v>
+        <v>45026</v>
       </c>
       <c r="AS5" s="10">
         <f ca="1">AR5+1</f>
-        <v>45013</v>
+        <v>45027</v>
       </c>
       <c r="AT5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45014</v>
+        <v>45028</v>
       </c>
       <c r="AU5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45015</v>
+        <v>45029</v>
       </c>
       <c r="AV5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45016</v>
+        <v>45030</v>
       </c>
       <c r="AW5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45017</v>
+        <v>45031</v>
       </c>
       <c r="AX5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45018</v>
+        <v>45032</v>
       </c>
       <c r="AY5" s="11">
         <f ca="1">AX5+1</f>
-        <v>45019</v>
+        <v>45033</v>
       </c>
       <c r="AZ5" s="10">
         <f ca="1">AY5+1</f>
-        <v>45020</v>
+        <v>45034</v>
       </c>
       <c r="BA5" s="10">
         <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
-        <v>45021</v>
+        <v>45035</v>
       </c>
       <c r="BB5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45022</v>
+        <v>45036</v>
       </c>
       <c r="BC5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45023</v>
+        <v>45037</v>
       </c>
       <c r="BD5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45024</v>
+        <v>45038</v>
       </c>
       <c r="BE5" s="12">
         <f t="shared" ca="1" si="1"/>
-        <v>45025</v>
+        <v>45039</v>
       </c>
       <c r="BF5" s="11">
         <f ca="1">BE5+1</f>
-        <v>45026</v>
+        <v>45040</v>
       </c>
       <c r="BG5" s="10">
         <f ca="1">BF5+1</f>
-        <v>45027</v>
+        <v>45041</v>
       </c>
       <c r="BH5" s="10">
         <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>45028</v>
+        <v>45042</v>
       </c>
       <c r="BI5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>45029</v>
+        <v>45043</v>
       </c>
       <c r="BJ5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>45030</v>
+        <v>45044</v>
       </c>
       <c r="BK5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>45031</v>
+        <v>45045</v>
       </c>
       <c r="BL5" s="12">
         <f t="shared" ca="1" si="2"/>
-        <v>45032</v>
+        <v>45046</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2571,13 +2577,17 @@
     </row>
     <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="59"/>
-      <c r="B13" s="81"/>
-      <c r="C13" s="82"/>
+      <c r="B13" s="81" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="82" t="s">
+        <v>51</v>
+      </c>
       <c r="D13" s="27">
-        <v>0</v>
+        <v>0.99</v>
       </c>
       <c r="E13" s="64">
-        <v>44620</v>
+        <v>44623</v>
       </c>
       <c r="F13" s="64">
         <v>44625</v>
@@ -2585,7 +2595,7 @@
       <c r="G13" s="17"/>
       <c r="H13" s="17">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I13" s="44"/>
       <c r="J13" s="44"/>

</xml_diff>

<commit_message>
Updated Gantt Chart Snapshot1
</commit_message>
<xml_diff>
--- a/Medical Al Disease Diagnostic Tool.Gantt.Chart.xlsx
+++ b/Medical Al Disease Diagnostic Tool.Gantt.Chart.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DCCCA8-BCF4-4019-B0E6-A37FE6B7A0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E444E7-9875-4F27-ADAE-70A4B477C1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="2805" windowWidth="25380" windowHeight="11385" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -910,6 +910,13 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -922,13 +929,6 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1499,7 +1499,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T14" sqref="T14"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1544,118 +1544,118 @@
       <c r="B3" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="89" t="s">
+      <c r="C3" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="90"/>
-      <c r="E3" s="88">
+      <c r="D3" s="86"/>
+      <c r="E3" s="91">
         <f ca="1">TODAY()</f>
-        <v>44990</v>
-      </c>
-      <c r="F3" s="88"/>
+        <v>44991</v>
+      </c>
+      <c r="F3" s="91"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="89" t="s">
+      <c r="C4" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="90"/>
+      <c r="D4" s="86"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="85">
+      <c r="I4" s="88">
         <f ca="1">I5</f>
         <v>44991</v>
       </c>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="87"/>
-      <c r="P4" s="85">
+      <c r="J4" s="89"/>
+      <c r="K4" s="89"/>
+      <c r="L4" s="89"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="90"/>
+      <c r="P4" s="88">
         <f ca="1">P5</f>
         <v>44998</v>
       </c>
-      <c r="Q4" s="86"/>
-      <c r="R4" s="86"/>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="86"/>
-      <c r="V4" s="87"/>
-      <c r="W4" s="85">
+      <c r="Q4" s="89"/>
+      <c r="R4" s="89"/>
+      <c r="S4" s="89"/>
+      <c r="T4" s="89"/>
+      <c r="U4" s="89"/>
+      <c r="V4" s="90"/>
+      <c r="W4" s="88">
         <f ca="1">W5</f>
         <v>45005</v>
       </c>
-      <c r="X4" s="86"/>
-      <c r="Y4" s="86"/>
-      <c r="Z4" s="86"/>
-      <c r="AA4" s="86"/>
-      <c r="AB4" s="86"/>
-      <c r="AC4" s="87"/>
-      <c r="AD4" s="85">
+      <c r="X4" s="89"/>
+      <c r="Y4" s="89"/>
+      <c r="Z4" s="89"/>
+      <c r="AA4" s="89"/>
+      <c r="AB4" s="89"/>
+      <c r="AC4" s="90"/>
+      <c r="AD4" s="88">
         <f ca="1">AD5</f>
         <v>45012</v>
       </c>
-      <c r="AE4" s="86"/>
-      <c r="AF4" s="86"/>
-      <c r="AG4" s="86"/>
-      <c r="AH4" s="86"/>
-      <c r="AI4" s="86"/>
-      <c r="AJ4" s="87"/>
-      <c r="AK4" s="85">
+      <c r="AE4" s="89"/>
+      <c r="AF4" s="89"/>
+      <c r="AG4" s="89"/>
+      <c r="AH4" s="89"/>
+      <c r="AI4" s="89"/>
+      <c r="AJ4" s="90"/>
+      <c r="AK4" s="88">
         <f ca="1">AK5</f>
         <v>45019</v>
       </c>
-      <c r="AL4" s="86"/>
-      <c r="AM4" s="86"/>
-      <c r="AN4" s="86"/>
-      <c r="AO4" s="86"/>
-      <c r="AP4" s="86"/>
-      <c r="AQ4" s="87"/>
-      <c r="AR4" s="85">
+      <c r="AL4" s="89"/>
+      <c r="AM4" s="89"/>
+      <c r="AN4" s="89"/>
+      <c r="AO4" s="89"/>
+      <c r="AP4" s="89"/>
+      <c r="AQ4" s="90"/>
+      <c r="AR4" s="88">
         <f ca="1">AR5</f>
         <v>45026</v>
       </c>
-      <c r="AS4" s="86"/>
-      <c r="AT4" s="86"/>
-      <c r="AU4" s="86"/>
-      <c r="AV4" s="86"/>
-      <c r="AW4" s="86"/>
-      <c r="AX4" s="87"/>
-      <c r="AY4" s="85">
+      <c r="AS4" s="89"/>
+      <c r="AT4" s="89"/>
+      <c r="AU4" s="89"/>
+      <c r="AV4" s="89"/>
+      <c r="AW4" s="89"/>
+      <c r="AX4" s="90"/>
+      <c r="AY4" s="88">
         <f ca="1">AY5</f>
         <v>45033</v>
       </c>
-      <c r="AZ4" s="86"/>
-      <c r="BA4" s="86"/>
-      <c r="BB4" s="86"/>
-      <c r="BC4" s="86"/>
-      <c r="BD4" s="86"/>
-      <c r="BE4" s="87"/>
-      <c r="BF4" s="85">
+      <c r="AZ4" s="89"/>
+      <c r="BA4" s="89"/>
+      <c r="BB4" s="89"/>
+      <c r="BC4" s="89"/>
+      <c r="BD4" s="89"/>
+      <c r="BE4" s="90"/>
+      <c r="BF4" s="88">
         <f ca="1">BF5</f>
         <v>45040</v>
       </c>
-      <c r="BG4" s="86"/>
-      <c r="BH4" s="86"/>
-      <c r="BI4" s="86"/>
-      <c r="BJ4" s="86"/>
-      <c r="BK4" s="86"/>
-      <c r="BL4" s="87"/>
+      <c r="BG4" s="89"/>
+      <c r="BH4" s="89"/>
+      <c r="BI4" s="89"/>
+      <c r="BJ4" s="89"/>
+      <c r="BK4" s="89"/>
+      <c r="BL4" s="90"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="91"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
       <c r="I5" s="11">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44991</v>
@@ -2359,7 +2359,7 @@
         <v>46</v>
       </c>
       <c r="D10" s="22">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E10" s="63">
         <v>44602</v>
@@ -4273,11 +4273,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4285,6 +4280,11 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
   <conditionalFormatting sqref="D7:D35">

</xml_diff>

<commit_message>
committing final Gantt chart
</commit_message>
<xml_diff>
--- a/Medical Al Disease Diagnostic Tool.Gantt.Chart.xlsx
+++ b/Medical Al Disease Diagnostic Tool.Gantt.Chart.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C86E11B-A9CC-446B-BD5B-422C5BBDD0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C570BE7-D6EE-4625-B677-C50A24E628FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1710" yWindow="1860" windowWidth="25380" windowHeight="11385" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -227,54 +227,6 @@
   </si>
   <si>
     <t>Mansoor, Kelvin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">File IO. Reading xlse data, and Display data </t>
-  </si>
-  <si>
-    <t>Kelvin, Mansoor</t>
-  </si>
-  <si>
-    <t>Update: Readme, Project Plan, Project Artifact. Create WiKi for new Snapshot</t>
-  </si>
-  <si>
-    <t>Web: Final Touchup and Refactor</t>
-  </si>
-  <si>
-    <t>User Testing and Bug Finding</t>
-  </si>
-  <si>
-    <t>Web: User Testing and Bug Finding</t>
-  </si>
-  <si>
-    <t>Final Touchups and Refactor</t>
-  </si>
-  <si>
-    <t>Code Implementation of Algorithm</t>
-  </si>
-  <si>
-    <t>Code Random and Display</t>
-  </si>
-  <si>
-    <t>A* Pathfindig Visualization</t>
-  </si>
-  <si>
-    <t>Web: Code Implementation of Algorithm</t>
-  </si>
-  <si>
-    <t>UI Design</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project Deployment </t>
-  </si>
-  <si>
-    <t>Project implementation</t>
-  </si>
-  <si>
-    <t>Web: UI Design</t>
-  </si>
-  <si>
-    <t>Adding Node</t>
   </si>
 </sst>
 </file>
@@ -1540,8 +1492,8 @@
   <dimension ref="A1:BL38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1592,7 +1544,7 @@
       <c r="D3" s="90"/>
       <c r="E3" s="88">
         <f ca="1">TODAY()</f>
-        <v>44992</v>
+        <v>44977</v>
       </c>
       <c r="F3" s="88"/>
     </row>
@@ -1609,7 +1561,7 @@
       </c>
       <c r="I4" s="85">
         <f ca="1">I5</f>
-        <v>44991</v>
+        <v>44977</v>
       </c>
       <c r="J4" s="86"/>
       <c r="K4" s="86"/>
@@ -1619,7 +1571,7 @@
       <c r="O4" s="87"/>
       <c r="P4" s="85">
         <f ca="1">P5</f>
-        <v>44998</v>
+        <v>44984</v>
       </c>
       <c r="Q4" s="86"/>
       <c r="R4" s="86"/>
@@ -1629,7 +1581,7 @@
       <c r="V4" s="87"/>
       <c r="W4" s="85">
         <f ca="1">W5</f>
-        <v>45005</v>
+        <v>44991</v>
       </c>
       <c r="X4" s="86"/>
       <c r="Y4" s="86"/>
@@ -1639,7 +1591,7 @@
       <c r="AC4" s="87"/>
       <c r="AD4" s="85">
         <f ca="1">AD5</f>
-        <v>45012</v>
+        <v>44998</v>
       </c>
       <c r="AE4" s="86"/>
       <c r="AF4" s="86"/>
@@ -1649,7 +1601,7 @@
       <c r="AJ4" s="87"/>
       <c r="AK4" s="85">
         <f ca="1">AK5</f>
-        <v>45019</v>
+        <v>45005</v>
       </c>
       <c r="AL4" s="86"/>
       <c r="AM4" s="86"/>
@@ -1659,7 +1611,7 @@
       <c r="AQ4" s="87"/>
       <c r="AR4" s="85">
         <f ca="1">AR5</f>
-        <v>45026</v>
+        <v>45012</v>
       </c>
       <c r="AS4" s="86"/>
       <c r="AT4" s="86"/>
@@ -1669,7 +1621,7 @@
       <c r="AX4" s="87"/>
       <c r="AY4" s="85">
         <f ca="1">AY5</f>
-        <v>45033</v>
+        <v>45019</v>
       </c>
       <c r="AZ4" s="86"/>
       <c r="BA4" s="86"/>
@@ -1679,7 +1631,7 @@
       <c r="BE4" s="87"/>
       <c r="BF4" s="85">
         <f ca="1">BF5</f>
-        <v>45040</v>
+        <v>45026</v>
       </c>
       <c r="BG4" s="86"/>
       <c r="BH4" s="86"/>
@@ -1700,227 +1652,227 @@
       <c r="G5" s="91"/>
       <c r="I5" s="11">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>44991</v>
+        <v>44977</v>
       </c>
       <c r="J5" s="10">
         <f ca="1">I5+1</f>
-        <v>44992</v>
+        <v>44978</v>
       </c>
       <c r="K5" s="10">
         <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
-        <v>44993</v>
+        <v>44979</v>
       </c>
       <c r="L5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44994</v>
+        <v>44980</v>
       </c>
       <c r="M5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44995</v>
+        <v>44981</v>
       </c>
       <c r="N5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>44996</v>
+        <v>44982</v>
       </c>
       <c r="O5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>44997</v>
+        <v>44983</v>
       </c>
       <c r="P5" s="11">
         <f ca="1">O5+1</f>
-        <v>44998</v>
+        <v>44984</v>
       </c>
       <c r="Q5" s="10">
         <f ca="1">P5+1</f>
-        <v>44999</v>
+        <v>44985</v>
       </c>
       <c r="R5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45000</v>
+        <v>44986</v>
       </c>
       <c r="S5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45001</v>
+        <v>44987</v>
       </c>
       <c r="T5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45002</v>
+        <v>44988</v>
       </c>
       <c r="U5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45003</v>
+        <v>44989</v>
       </c>
       <c r="V5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45004</v>
+        <v>44990</v>
       </c>
       <c r="W5" s="11">
         <f ca="1">V5+1</f>
-        <v>45005</v>
+        <v>44991</v>
       </c>
       <c r="X5" s="10">
         <f ca="1">W5+1</f>
-        <v>45006</v>
+        <v>44992</v>
       </c>
       <c r="Y5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45007</v>
+        <v>44993</v>
       </c>
       <c r="Z5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45008</v>
+        <v>44994</v>
       </c>
       <c r="AA5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45009</v>
+        <v>44995</v>
       </c>
       <c r="AB5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45010</v>
+        <v>44996</v>
       </c>
       <c r="AC5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45011</v>
+        <v>44997</v>
       </c>
       <c r="AD5" s="11">
         <f ca="1">AC5+1</f>
-        <v>45012</v>
+        <v>44998</v>
       </c>
       <c r="AE5" s="10">
         <f ca="1">AD5+1</f>
-        <v>45013</v>
+        <v>44999</v>
       </c>
       <c r="AF5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45014</v>
+        <v>45000</v>
       </c>
       <c r="AG5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45015</v>
+        <v>45001</v>
       </c>
       <c r="AH5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45016</v>
+        <v>45002</v>
       </c>
       <c r="AI5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45017</v>
+        <v>45003</v>
       </c>
       <c r="AJ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45018</v>
+        <v>45004</v>
       </c>
       <c r="AK5" s="11">
         <f ca="1">AJ5+1</f>
-        <v>45019</v>
+        <v>45005</v>
       </c>
       <c r="AL5" s="10">
         <f ca="1">AK5+1</f>
-        <v>45020</v>
+        <v>45006</v>
       </c>
       <c r="AM5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45021</v>
+        <v>45007</v>
       </c>
       <c r="AN5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45022</v>
+        <v>45008</v>
       </c>
       <c r="AO5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45023</v>
+        <v>45009</v>
       </c>
       <c r="AP5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45024</v>
+        <v>45010</v>
       </c>
       <c r="AQ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45025</v>
+        <v>45011</v>
       </c>
       <c r="AR5" s="11">
         <f ca="1">AQ5+1</f>
-        <v>45026</v>
+        <v>45012</v>
       </c>
       <c r="AS5" s="10">
         <f ca="1">AR5+1</f>
-        <v>45027</v>
+        <v>45013</v>
       </c>
       <c r="AT5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45028</v>
+        <v>45014</v>
       </c>
       <c r="AU5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45029</v>
+        <v>45015</v>
       </c>
       <c r="AV5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45030</v>
+        <v>45016</v>
       </c>
       <c r="AW5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45031</v>
+        <v>45017</v>
       </c>
       <c r="AX5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45032</v>
+        <v>45018</v>
       </c>
       <c r="AY5" s="11">
         <f ca="1">AX5+1</f>
-        <v>45033</v>
+        <v>45019</v>
       </c>
       <c r="AZ5" s="10">
         <f ca="1">AY5+1</f>
-        <v>45034</v>
+        <v>45020</v>
       </c>
       <c r="BA5" s="10">
         <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
-        <v>45035</v>
+        <v>45021</v>
       </c>
       <c r="BB5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45036</v>
+        <v>45022</v>
       </c>
       <c r="BC5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45037</v>
+        <v>45023</v>
       </c>
       <c r="BD5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45038</v>
+        <v>45024</v>
       </c>
       <c r="BE5" s="12">
         <f t="shared" ca="1" si="1"/>
-        <v>45039</v>
+        <v>45025</v>
       </c>
       <c r="BF5" s="11">
         <f ca="1">BE5+1</f>
-        <v>45040</v>
+        <v>45026</v>
       </c>
       <c r="BG5" s="10">
         <f ca="1">BF5+1</f>
-        <v>45041</v>
+        <v>45027</v>
       </c>
       <c r="BH5" s="10">
         <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>45042</v>
+        <v>45028</v>
       </c>
       <c r="BI5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>45043</v>
+        <v>45029</v>
       </c>
       <c r="BJ5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>45044</v>
+        <v>45030</v>
       </c>
       <c r="BK5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>45045</v>
+        <v>45031</v>
       </c>
       <c r="BL5" s="12">
         <f t="shared" ca="1" si="2"/>
-        <v>45046</v>
+        <v>45032</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2401,7 +2353,7 @@
         <v>46</v>
       </c>
       <c r="D10" s="22">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E10" s="63">
         <v>44602</v>
@@ -2619,17 +2571,13 @@
     </row>
     <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="59"/>
-      <c r="B13" s="81" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="82" t="s">
-        <v>52</v>
-      </c>
+      <c r="B13" s="81"/>
+      <c r="C13" s="82"/>
       <c r="D13" s="27">
-        <v>0.99</v>
+        <v>0</v>
       </c>
       <c r="E13" s="64">
-        <v>44623</v>
+        <v>44620</v>
       </c>
       <c r="F13" s="64">
         <v>44625</v>
@@ -2637,7 +2585,7 @@
       <c r="G13" s="17"/>
       <c r="H13" s="17">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I13" s="44"/>
       <c r="J13" s="44"/>
@@ -2698,12 +2646,8 @@
     </row>
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="59"/>
-      <c r="B14" s="81" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" s="82" t="s">
-        <v>46</v>
-      </c>
+      <c r="B14" s="81"/>
+      <c r="C14" s="82"/>
       <c r="D14" s="27">
         <v>0</v>
       </c>
@@ -2774,12 +2718,8 @@
     </row>
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="59"/>
-      <c r="B15" s="81" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="82" t="s">
-        <v>46</v>
-      </c>
+      <c r="B15" s="81"/>
+      <c r="C15" s="82"/>
       <c r="D15" s="27">
         <v>0</v>
       </c>
@@ -2850,12 +2790,8 @@
     </row>
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="59"/>
-      <c r="B16" s="81" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="82" t="s">
-        <v>46</v>
-      </c>
+      <c r="B16" s="81"/>
+      <c r="C16" s="82"/>
       <c r="D16" s="27">
         <v>0</v>
       </c>
@@ -2926,12 +2862,8 @@
     </row>
     <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="59"/>
-      <c r="B17" s="81" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="82" t="s">
-        <v>46</v>
-      </c>
+      <c r="B17" s="81"/>
+      <c r="C17" s="82"/>
       <c r="D17" s="27">
         <v>0</v>
       </c>
@@ -3002,12 +2934,8 @@
     </row>
     <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="58"/>
-      <c r="B18" s="81" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="82" t="s">
-        <v>38</v>
-      </c>
+      <c r="B18" s="81"/>
+      <c r="C18" s="82"/>
       <c r="D18" s="27">
         <v>0</v>
       </c>
@@ -3154,12 +3082,8 @@
     </row>
     <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="58"/>
-      <c r="B20" s="83" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="72" t="s">
-        <v>46</v>
-      </c>
+      <c r="B20" s="83"/>
+      <c r="C20" s="72"/>
       <c r="D20" s="32">
         <v>0</v>
       </c>
@@ -3234,9 +3158,7 @@
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="58"/>
       <c r="B21" s="83"/>
-      <c r="C21" s="72" t="s">
-        <v>46</v>
-      </c>
+      <c r="C21" s="72"/>
       <c r="D21" s="32">
         <v>0</v>
       </c>
@@ -3307,12 +3229,8 @@
     </row>
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="58"/>
-      <c r="B22" s="83" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="72" t="s">
-        <v>46</v>
-      </c>
+      <c r="B22" s="83"/>
+      <c r="C22" s="72"/>
       <c r="D22" s="32">
         <v>0</v>
       </c>
@@ -3383,12 +3301,8 @@
     </row>
     <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="58"/>
-      <c r="B23" s="83" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="72" t="s">
-        <v>46</v>
-      </c>
+      <c r="B23" s="83"/>
+      <c r="C23" s="72"/>
       <c r="D23" s="32">
         <v>0</v>
       </c>
@@ -3459,12 +3373,8 @@
     </row>
     <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="58"/>
-      <c r="B24" s="83" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="72" t="s">
-        <v>46</v>
-      </c>
+      <c r="B24" s="83"/>
+      <c r="C24" s="72"/>
       <c r="D24" s="32">
         <v>0</v>
       </c>
@@ -3535,12 +3445,8 @@
     </row>
     <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="58"/>
-      <c r="B25" s="83" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="72" t="s">
-        <v>46</v>
-      </c>
+      <c r="B25" s="83"/>
+      <c r="C25" s="72"/>
       <c r="D25" s="32">
         <v>0</v>
       </c>
@@ -3611,12 +3517,8 @@
     </row>
     <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="58"/>
-      <c r="B26" s="83" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="72" t="s">
-        <v>38</v>
-      </c>
+      <c r="B26" s="83"/>
+      <c r="C26" s="72"/>
       <c r="D26" s="32">
         <v>0</v>
       </c>
@@ -3760,12 +3662,8 @@
     </row>
     <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="58"/>
-      <c r="B28" s="84" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="74" t="s">
-        <v>46</v>
-      </c>
+      <c r="B28" s="84"/>
+      <c r="C28" s="74"/>
       <c r="D28" s="37">
         <v>0</v>
       </c>
@@ -3839,12 +3737,8 @@
     </row>
     <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="58"/>
-      <c r="B29" s="84" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="74" t="s">
-        <v>46</v>
-      </c>
+      <c r="B29" s="84"/>
+      <c r="C29" s="74"/>
       <c r="D29" s="37">
         <v>0</v>
       </c>
@@ -3915,12 +3809,8 @@
     </row>
     <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="58"/>
-      <c r="B30" s="84" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" s="74" t="s">
-        <v>46</v>
-      </c>
+      <c r="B30" s="84"/>
+      <c r="C30" s="74"/>
       <c r="D30" s="37">
         <v>0</v>
       </c>
@@ -3991,12 +3881,8 @@
     </row>
     <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="58"/>
-      <c r="B31" s="84" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" s="74" t="s">
-        <v>46</v>
-      </c>
+      <c r="B31" s="84"/>
+      <c r="C31" s="74"/>
       <c r="D31" s="37">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Detected outliers using the Z-score method
</commit_message>
<xml_diff>
--- a/Medical Al Disease Diagnostic Tool.Gantt.Chart.xlsx
+++ b/Medical Al Disease Diagnostic Tool.Gantt.Chart.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D1D038-CB74-4BA1-846F-1CFDB32F1A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B6883C-A107-4742-9306-F92F8D6E8761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="760" windowWidth="26700" windowHeight="17440" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -1004,6 +1004,13 @@
     <xf numFmtId="0" fontId="27" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1016,13 +1023,6 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1592,25 +1592,25 @@
   <dimension ref="A1:BL43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="57" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" hidden="1" customWidth="1"/>
-    <col min="9" max="64" width="2.42578125" customWidth="1"/>
-    <col min="69" max="70" width="10.28515625"/>
+    <col min="1" max="1" width="2.6640625" style="57" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" customWidth="1"/>
+    <col min="8" max="8" width="6.1640625" hidden="1" customWidth="1"/>
+    <col min="9" max="64" width="2.5" customWidth="1"/>
+    <col min="69" max="70" width="10.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="58"/>
       <c r="B1" s="78" t="s">
         <v>40</v>
@@ -1622,7 +1622,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="14"/>
     </row>
-    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="57" t="s">
         <v>23</v>
       </c>
@@ -1631,125 +1631,125 @@
       </c>
       <c r="I2" s="60"/>
     </row>
-    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="57" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="87" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="92"/>
-      <c r="E3" s="90">
+      <c r="D3" s="88"/>
+      <c r="E3" s="93">
         <f ca="1">TODAY()</f>
-        <v>45018</v>
-      </c>
-      <c r="F3" s="90"/>
-    </row>
-    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45021</v>
+      </c>
+      <c r="F3" s="93"/>
+    </row>
+    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="91" t="s">
+      <c r="C4" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="92"/>
+      <c r="D4" s="88"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="87">
+      <c r="I4" s="90">
         <f ca="1">I5</f>
         <v>45019</v>
       </c>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="89"/>
-      <c r="P4" s="87">
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="91"/>
+      <c r="O4" s="92"/>
+      <c r="P4" s="90">
         <f ca="1">P5</f>
         <v>45026</v>
       </c>
-      <c r="Q4" s="88"/>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="88"/>
-      <c r="V4" s="89"/>
-      <c r="W4" s="87">
+      <c r="Q4" s="91"/>
+      <c r="R4" s="91"/>
+      <c r="S4" s="91"/>
+      <c r="T4" s="91"/>
+      <c r="U4" s="91"/>
+      <c r="V4" s="92"/>
+      <c r="W4" s="90">
         <f ca="1">W5</f>
         <v>45033</v>
       </c>
-      <c r="X4" s="88"/>
-      <c r="Y4" s="88"/>
-      <c r="Z4" s="88"/>
-      <c r="AA4" s="88"/>
-      <c r="AB4" s="88"/>
-      <c r="AC4" s="89"/>
-      <c r="AD4" s="87">
+      <c r="X4" s="91"/>
+      <c r="Y4" s="91"/>
+      <c r="Z4" s="91"/>
+      <c r="AA4" s="91"/>
+      <c r="AB4" s="91"/>
+      <c r="AC4" s="92"/>
+      <c r="AD4" s="90">
         <f ca="1">AD5</f>
         <v>45040</v>
       </c>
-      <c r="AE4" s="88"/>
-      <c r="AF4" s="88"/>
-      <c r="AG4" s="88"/>
-      <c r="AH4" s="88"/>
-      <c r="AI4" s="88"/>
-      <c r="AJ4" s="89"/>
-      <c r="AK4" s="87">
+      <c r="AE4" s="91"/>
+      <c r="AF4" s="91"/>
+      <c r="AG4" s="91"/>
+      <c r="AH4" s="91"/>
+      <c r="AI4" s="91"/>
+      <c r="AJ4" s="92"/>
+      <c r="AK4" s="90">
         <f ca="1">AK5</f>
         <v>45047</v>
       </c>
-      <c r="AL4" s="88"/>
-      <c r="AM4" s="88"/>
-      <c r="AN4" s="88"/>
-      <c r="AO4" s="88"/>
-      <c r="AP4" s="88"/>
-      <c r="AQ4" s="89"/>
-      <c r="AR4" s="87">
+      <c r="AL4" s="91"/>
+      <c r="AM4" s="91"/>
+      <c r="AN4" s="91"/>
+      <c r="AO4" s="91"/>
+      <c r="AP4" s="91"/>
+      <c r="AQ4" s="92"/>
+      <c r="AR4" s="90">
         <f ca="1">AR5</f>
         <v>45054</v>
       </c>
-      <c r="AS4" s="88"/>
-      <c r="AT4" s="88"/>
-      <c r="AU4" s="88"/>
-      <c r="AV4" s="88"/>
-      <c r="AW4" s="88"/>
-      <c r="AX4" s="89"/>
-      <c r="AY4" s="87">
+      <c r="AS4" s="91"/>
+      <c r="AT4" s="91"/>
+      <c r="AU4" s="91"/>
+      <c r="AV4" s="91"/>
+      <c r="AW4" s="91"/>
+      <c r="AX4" s="92"/>
+      <c r="AY4" s="90">
         <f ca="1">AY5</f>
         <v>45061</v>
       </c>
-      <c r="AZ4" s="88"/>
-      <c r="BA4" s="88"/>
-      <c r="BB4" s="88"/>
-      <c r="BC4" s="88"/>
-      <c r="BD4" s="88"/>
-      <c r="BE4" s="89"/>
-      <c r="BF4" s="87">
+      <c r="AZ4" s="91"/>
+      <c r="BA4" s="91"/>
+      <c r="BB4" s="91"/>
+      <c r="BC4" s="91"/>
+      <c r="BD4" s="91"/>
+      <c r="BE4" s="92"/>
+      <c r="BF4" s="90">
         <f ca="1">BF5</f>
         <v>45068</v>
       </c>
-      <c r="BG4" s="88"/>
-      <c r="BH4" s="88"/>
-      <c r="BI4" s="88"/>
-      <c r="BJ4" s="88"/>
-      <c r="BK4" s="88"/>
-      <c r="BL4" s="89"/>
-    </row>
-    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BG4" s="91"/>
+      <c r="BH4" s="91"/>
+      <c r="BI4" s="91"/>
+      <c r="BJ4" s="91"/>
+      <c r="BK4" s="91"/>
+      <c r="BL4" s="92"/>
+    </row>
+    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="89"/>
       <c r="I5" s="11">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>45019</v>
@@ -1975,7 +1975,7 @@
         <v>45074</v>
       </c>
     </row>
-    <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
         <v>31</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="57" t="s">
         <v>27</v>
       </c>
@@ -2290,7 +2290,7 @@
       <c r="BK7" s="44"/>
       <c r="BL7" s="44"/>
     </row>
-    <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
         <v>32</v>
       </c>
@@ -2365,7 +2365,7 @@
       <c r="BK8" s="44"/>
       <c r="BL8" s="44"/>
     </row>
-    <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
         <v>33</v>
       </c>
@@ -2446,7 +2446,7 @@
       <c r="BK9" s="44"/>
       <c r="BL9" s="44"/>
     </row>
-    <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="58"/>
       <c r="B10" s="79" t="s">
         <v>45</v>
@@ -2522,7 +2522,7 @@
       <c r="BK10" s="44"/>
       <c r="BL10" s="44"/>
     </row>
-    <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="58"/>
       <c r="B11" s="79" t="s">
         <v>43</v>
@@ -2598,7 +2598,7 @@
       <c r="BK11" s="44"/>
       <c r="BL11" s="44"/>
     </row>
-    <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
         <v>34</v>
       </c>
@@ -2675,7 +2675,7 @@
       <c r="BK12" s="44"/>
       <c r="BL12" s="44"/>
     </row>
-    <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="58"/>
       <c r="B13" s="80" t="s">
         <v>63</v>
@@ -2754,7 +2754,7 @@
       <c r="BK13" s="44"/>
       <c r="BL13" s="44"/>
     </row>
-    <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="58"/>
       <c r="B14" s="80" t="s">
         <v>64</v>
@@ -2830,7 +2830,7 @@
       <c r="BK14" s="44"/>
       <c r="BL14" s="44"/>
     </row>
-    <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="58"/>
       <c r="B15" s="80" t="s">
         <v>65</v>
@@ -2839,7 +2839,7 @@
         <v>61</v>
       </c>
       <c r="D15" s="27">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E15" s="63">
         <v>44997</v>
@@ -2906,13 +2906,13 @@
       <c r="BK15" s="44"/>
       <c r="BL15" s="44"/>
     </row>
-    <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="58"/>
       <c r="B16" s="80" t="s">
         <v>66</v>
       </c>
       <c r="C16" s="81" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D16" s="27">
         <v>1</v>
@@ -2982,13 +2982,13 @@
       <c r="BK16" s="44"/>
       <c r="BL16" s="44"/>
     </row>
-    <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="58"/>
       <c r="B17" s="80" t="s">
         <v>67</v>
       </c>
       <c r="C17" s="81" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D17" s="27">
         <v>1</v>
@@ -3058,7 +3058,7 @@
       <c r="BK17" s="44"/>
       <c r="BL17" s="44"/>
     </row>
-    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="57"/>
       <c r="B18" s="80" t="s">
         <v>68</v>
@@ -3137,7 +3137,7 @@
       <c r="BK18" s="44"/>
       <c r="BL18" s="44"/>
     </row>
-    <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="57" t="s">
         <v>24</v>
       </c>
@@ -3216,7 +3216,7 @@
       <c r="BK19" s="44"/>
       <c r="BL19" s="44"/>
     </row>
-    <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="57"/>
       <c r="B20" s="80" t="s">
         <v>74</v>
@@ -3293,7 +3293,7 @@
       <c r="BK20" s="44"/>
       <c r="BL20" s="44"/>
     </row>
-    <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="57"/>
       <c r="B21" s="80" t="s">
         <v>69</v>
@@ -3367,7 +3367,7 @@
       <c r="BK21" s="44"/>
       <c r="BL21" s="44"/>
     </row>
-    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="57"/>
       <c r="B22" s="28" t="s">
         <v>70</v>
@@ -3441,7 +3441,7 @@
       <c r="BK22" s="44"/>
       <c r="BL22" s="44"/>
     </row>
-    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="57"/>
       <c r="B23" s="82" t="s">
         <v>71</v>
@@ -3515,7 +3515,7 @@
       <c r="BK23" s="44"/>
       <c r="BL23" s="44"/>
     </row>
-    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="57"/>
       <c r="B24" s="82" t="s">
         <v>59</v>
@@ -3589,7 +3589,7 @@
       <c r="BK24" s="44"/>
       <c r="BL24" s="44"/>
     </row>
-    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="57"/>
       <c r="B25" s="82" t="s">
         <v>50</v>
@@ -3663,7 +3663,7 @@
       <c r="BK25" s="44"/>
       <c r="BL25" s="44"/>
     </row>
-    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="57"/>
       <c r="B26" s="82" t="s">
         <v>72</v>
@@ -3737,7 +3737,7 @@
       <c r="BK26" s="44"/>
       <c r="BL26" s="44"/>
     </row>
-    <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="57"/>
       <c r="B27" s="82" t="s">
         <v>53</v>
@@ -3811,7 +3811,7 @@
       <c r="BK27" s="44"/>
       <c r="BL27" s="44"/>
     </row>
-    <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="57" t="s">
         <v>24</v>
       </c>
@@ -3890,7 +3890,7 @@
       <c r="BK28" s="44"/>
       <c r="BL28" s="44"/>
     </row>
-    <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="57"/>
       <c r="B29" s="82" t="s">
         <v>57</v>
@@ -3967,7 +3967,7 @@
       <c r="BK29" s="44"/>
       <c r="BL29" s="44"/>
     </row>
-    <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="57"/>
       <c r="B30" s="82" t="s">
         <v>58</v>
@@ -4041,7 +4041,7 @@
       <c r="BK30" s="44"/>
       <c r="BL30" s="44"/>
     </row>
-    <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="57"/>
       <c r="B31" s="33" t="s">
         <v>36</v>
@@ -4113,7 +4113,7 @@
       <c r="BK31" s="44"/>
       <c r="BL31" s="44"/>
     </row>
-    <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="57"/>
       <c r="B32" s="83" t="s">
         <v>55</v>
@@ -4189,7 +4189,7 @@
       <c r="BK32" s="44"/>
       <c r="BL32" s="44"/>
     </row>
-    <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="57"/>
       <c r="B33" s="83" t="s">
         <v>51</v>
@@ -4263,7 +4263,7 @@
       <c r="BK33" s="44"/>
       <c r="BL33" s="44"/>
     </row>
-    <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="57"/>
       <c r="B34" s="83" t="s">
         <v>56</v>
@@ -4337,7 +4337,7 @@
       <c r="BK34" s="44"/>
       <c r="BL34" s="44"/>
     </row>
-    <row r="35" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="57"/>
       <c r="B35" s="83" t="s">
         <v>52</v>
@@ -4414,7 +4414,7 @@
       <c r="BK35" s="44"/>
       <c r="BL35" s="44"/>
     </row>
-    <row r="36" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="57" t="s">
         <v>26</v>
       </c>
@@ -4495,7 +4495,7 @@
       <c r="BK36" s="44"/>
       <c r="BL36" s="44"/>
     </row>
-    <row r="37" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="58" t="s">
         <v>25</v>
       </c>
@@ -4576,7 +4576,7 @@
       <c r="BK37" s="45"/>
       <c r="BL37" s="45"/>
     </row>
-    <row r="38" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="83" t="s">
         <v>48</v>
       </c>
@@ -4594,14 +4594,14 @@
       </c>
       <c r="G38" s="6"/>
     </row>
-    <row r="39" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="75"/>
       <c r="C39" s="74"/>
       <c r="D39" s="16"/>
       <c r="E39" s="66"/>
       <c r="F39" s="66"/>
     </row>
-    <row r="40" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="38" t="s">
         <v>0</v>
       </c>
@@ -4610,20 +4610,15 @@
       <c r="E40" s="41"/>
       <c r="F40" s="42"/>
     </row>
-    <row r="42" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C42" s="14"/>
       <c r="F42" s="59"/>
     </row>
-    <row r="43" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C43" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4631,6 +4626,11 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
   <conditionalFormatting sqref="D7:D40">
@@ -4701,31 +4701,31 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="87.140625" style="47" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="87.1640625" style="47" customWidth="1"/>
+    <col min="2" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:2" s="49" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="49" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="48" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="48"/>
     </row>
-    <row r="3" spans="1:2" s="53" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="53" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="54" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="54"/>
     </row>
-    <row r="4" spans="1:2" s="50" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" s="50" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A4" s="51" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="74" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="52" t="s">
         <v>19</v>
       </c>
@@ -4735,42 +4735,42 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="47" customFormat="1" ht="204.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" s="47" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="56" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="50" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2" s="50" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A8" s="51" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="52" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="47" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" s="47" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="55" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="50" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:2" s="50" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A11" s="51" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="52" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="47" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" s="47" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="55" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="50" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" s="50" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A14" s="51" t="s">
         <v>13</v>
       </c>
@@ -4780,7 +4780,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="52" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
added a feature that will allow users to select whether to conduct diagnostics with or without outliers.
</commit_message>
<xml_diff>
--- a/Medical Al Disease Diagnostic Tool.Gantt.Chart.xlsx
+++ b/Medical Al Disease Diagnostic Tool.Gantt.Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B861C9-FA21-7941-9E4B-56CCA3BC2075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46AF60B2-EE29-4649-B00B-15C435C78577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="760" windowWidth="26700" windowHeight="17440" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1001,6 +1001,18 @@
     <xf numFmtId="0" fontId="27" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -1008,18 +1020,6 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1590,7 +1590,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1635,341 +1635,341 @@
       <c r="B3" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="87" t="s">
+      <c r="C3" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="88"/>
-      <c r="E3" s="93">
+      <c r="D3" s="92"/>
+      <c r="E3" s="90">
         <f ca="1">TODAY()</f>
-        <v>45022</v>
-      </c>
-      <c r="F3" s="93"/>
+        <v>45025</v>
+      </c>
+      <c r="F3" s="90"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="88"/>
+      <c r="D4" s="92"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="90">
+      <c r="I4" s="87">
         <f ca="1">I5</f>
-        <v>45019</v>
-      </c>
-      <c r="J4" s="91"/>
-      <c r="K4" s="91"/>
-      <c r="L4" s="91"/>
-      <c r="M4" s="91"/>
-      <c r="N4" s="91"/>
-      <c r="O4" s="92"/>
-      <c r="P4" s="90">
+        <v>45026</v>
+      </c>
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
+      <c r="M4" s="88"/>
+      <c r="N4" s="88"/>
+      <c r="O4" s="89"/>
+      <c r="P4" s="87">
         <f ca="1">P5</f>
-        <v>45026</v>
-      </c>
-      <c r="Q4" s="91"/>
-      <c r="R4" s="91"/>
-      <c r="S4" s="91"/>
-      <c r="T4" s="91"/>
-      <c r="U4" s="91"/>
-      <c r="V4" s="92"/>
-      <c r="W4" s="90">
+        <v>45033</v>
+      </c>
+      <c r="Q4" s="88"/>
+      <c r="R4" s="88"/>
+      <c r="S4" s="88"/>
+      <c r="T4" s="88"/>
+      <c r="U4" s="88"/>
+      <c r="V4" s="89"/>
+      <c r="W4" s="87">
         <f ca="1">W5</f>
-        <v>45033</v>
-      </c>
-      <c r="X4" s="91"/>
-      <c r="Y4" s="91"/>
-      <c r="Z4" s="91"/>
-      <c r="AA4" s="91"/>
-      <c r="AB4" s="91"/>
-      <c r="AC4" s="92"/>
-      <c r="AD4" s="90">
+        <v>45040</v>
+      </c>
+      <c r="X4" s="88"/>
+      <c r="Y4" s="88"/>
+      <c r="Z4" s="88"/>
+      <c r="AA4" s="88"/>
+      <c r="AB4" s="88"/>
+      <c r="AC4" s="89"/>
+      <c r="AD4" s="87">
         <f ca="1">AD5</f>
-        <v>45040</v>
-      </c>
-      <c r="AE4" s="91"/>
-      <c r="AF4" s="91"/>
-      <c r="AG4" s="91"/>
-      <c r="AH4" s="91"/>
-      <c r="AI4" s="91"/>
-      <c r="AJ4" s="92"/>
-      <c r="AK4" s="90">
+        <v>45047</v>
+      </c>
+      <c r="AE4" s="88"/>
+      <c r="AF4" s="88"/>
+      <c r="AG4" s="88"/>
+      <c r="AH4" s="88"/>
+      <c r="AI4" s="88"/>
+      <c r="AJ4" s="89"/>
+      <c r="AK4" s="87">
         <f ca="1">AK5</f>
-        <v>45047</v>
-      </c>
-      <c r="AL4" s="91"/>
-      <c r="AM4" s="91"/>
-      <c r="AN4" s="91"/>
-      <c r="AO4" s="91"/>
-      <c r="AP4" s="91"/>
-      <c r="AQ4" s="92"/>
-      <c r="AR4" s="90">
+        <v>45054</v>
+      </c>
+      <c r="AL4" s="88"/>
+      <c r="AM4" s="88"/>
+      <c r="AN4" s="88"/>
+      <c r="AO4" s="88"/>
+      <c r="AP4" s="88"/>
+      <c r="AQ4" s="89"/>
+      <c r="AR4" s="87">
         <f ca="1">AR5</f>
-        <v>45054</v>
-      </c>
-      <c r="AS4" s="91"/>
-      <c r="AT4" s="91"/>
-      <c r="AU4" s="91"/>
-      <c r="AV4" s="91"/>
-      <c r="AW4" s="91"/>
-      <c r="AX4" s="92"/>
-      <c r="AY4" s="90">
+        <v>45061</v>
+      </c>
+      <c r="AS4" s="88"/>
+      <c r="AT4" s="88"/>
+      <c r="AU4" s="88"/>
+      <c r="AV4" s="88"/>
+      <c r="AW4" s="88"/>
+      <c r="AX4" s="89"/>
+      <c r="AY4" s="87">
         <f ca="1">AY5</f>
-        <v>45061</v>
-      </c>
-      <c r="AZ4" s="91"/>
-      <c r="BA4" s="91"/>
-      <c r="BB4" s="91"/>
-      <c r="BC4" s="91"/>
-      <c r="BD4" s="91"/>
-      <c r="BE4" s="92"/>
-      <c r="BF4" s="90">
+        <v>45068</v>
+      </c>
+      <c r="AZ4" s="88"/>
+      <c r="BA4" s="88"/>
+      <c r="BB4" s="88"/>
+      <c r="BC4" s="88"/>
+      <c r="BD4" s="88"/>
+      <c r="BE4" s="89"/>
+      <c r="BF4" s="87">
         <f ca="1">BF5</f>
-        <v>45068</v>
-      </c>
-      <c r="BG4" s="91"/>
-      <c r="BH4" s="91"/>
-      <c r="BI4" s="91"/>
-      <c r="BJ4" s="91"/>
-      <c r="BK4" s="91"/>
-      <c r="BL4" s="92"/>
+        <v>45075</v>
+      </c>
+      <c r="BG4" s="88"/>
+      <c r="BH4" s="88"/>
+      <c r="BI4" s="88"/>
+      <c r="BJ4" s="88"/>
+      <c r="BK4" s="88"/>
+      <c r="BL4" s="89"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
       <c r="I5" s="11">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>45019</v>
+        <v>45026</v>
       </c>
       <c r="J5" s="10">
         <f ca="1">I5+1</f>
-        <v>45020</v>
+        <v>45027</v>
       </c>
       <c r="K5" s="10">
         <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
-        <v>45021</v>
+        <v>45028</v>
       </c>
       <c r="L5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45022</v>
+        <v>45029</v>
       </c>
       <c r="M5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45023</v>
+        <v>45030</v>
       </c>
       <c r="N5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45024</v>
+        <v>45031</v>
       </c>
       <c r="O5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45025</v>
+        <v>45032</v>
       </c>
       <c r="P5" s="11">
         <f ca="1">O5+1</f>
-        <v>45026</v>
+        <v>45033</v>
       </c>
       <c r="Q5" s="10">
         <f ca="1">P5+1</f>
-        <v>45027</v>
+        <v>45034</v>
       </c>
       <c r="R5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45028</v>
+        <v>45035</v>
       </c>
       <c r="S5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45029</v>
+        <v>45036</v>
       </c>
       <c r="T5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45030</v>
+        <v>45037</v>
       </c>
       <c r="U5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45031</v>
+        <v>45038</v>
       </c>
       <c r="V5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45032</v>
+        <v>45039</v>
       </c>
       <c r="W5" s="11">
         <f ca="1">V5+1</f>
-        <v>45033</v>
+        <v>45040</v>
       </c>
       <c r="X5" s="10">
         <f ca="1">W5+1</f>
-        <v>45034</v>
+        <v>45041</v>
       </c>
       <c r="Y5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45035</v>
+        <v>45042</v>
       </c>
       <c r="Z5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45036</v>
+        <v>45043</v>
       </c>
       <c r="AA5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45037</v>
+        <v>45044</v>
       </c>
       <c r="AB5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45038</v>
+        <v>45045</v>
       </c>
       <c r="AC5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45039</v>
+        <v>45046</v>
       </c>
       <c r="AD5" s="11">
         <f ca="1">AC5+1</f>
-        <v>45040</v>
+        <v>45047</v>
       </c>
       <c r="AE5" s="10">
         <f ca="1">AD5+1</f>
-        <v>45041</v>
+        <v>45048</v>
       </c>
       <c r="AF5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45042</v>
+        <v>45049</v>
       </c>
       <c r="AG5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45043</v>
+        <v>45050</v>
       </c>
       <c r="AH5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45044</v>
+        <v>45051</v>
       </c>
       <c r="AI5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45045</v>
+        <v>45052</v>
       </c>
       <c r="AJ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45046</v>
+        <v>45053</v>
       </c>
       <c r="AK5" s="11">
         <f ca="1">AJ5+1</f>
-        <v>45047</v>
+        <v>45054</v>
       </c>
       <c r="AL5" s="10">
         <f ca="1">AK5+1</f>
-        <v>45048</v>
+        <v>45055</v>
       </c>
       <c r="AM5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45049</v>
+        <v>45056</v>
       </c>
       <c r="AN5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45050</v>
+        <v>45057</v>
       </c>
       <c r="AO5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45051</v>
+        <v>45058</v>
       </c>
       <c r="AP5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45052</v>
+        <v>45059</v>
       </c>
       <c r="AQ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45053</v>
+        <v>45060</v>
       </c>
       <c r="AR5" s="11">
         <f ca="1">AQ5+1</f>
-        <v>45054</v>
+        <v>45061</v>
       </c>
       <c r="AS5" s="10">
         <f ca="1">AR5+1</f>
-        <v>45055</v>
+        <v>45062</v>
       </c>
       <c r="AT5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45056</v>
+        <v>45063</v>
       </c>
       <c r="AU5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45057</v>
+        <v>45064</v>
       </c>
       <c r="AV5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45058</v>
+        <v>45065</v>
       </c>
       <c r="AW5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>45059</v>
+        <v>45066</v>
       </c>
       <c r="AX5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45060</v>
+        <v>45067</v>
       </c>
       <c r="AY5" s="11">
         <f ca="1">AX5+1</f>
-        <v>45061</v>
+        <v>45068</v>
       </c>
       <c r="AZ5" s="10">
         <f ca="1">AY5+1</f>
-        <v>45062</v>
+        <v>45069</v>
       </c>
       <c r="BA5" s="10">
         <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
-        <v>45063</v>
+        <v>45070</v>
       </c>
       <c r="BB5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45064</v>
+        <v>45071</v>
       </c>
       <c r="BC5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45065</v>
+        <v>45072</v>
       </c>
       <c r="BD5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45066</v>
+        <v>45073</v>
       </c>
       <c r="BE5" s="12">
         <f t="shared" ca="1" si="1"/>
-        <v>45067</v>
+        <v>45074</v>
       </c>
       <c r="BF5" s="11">
         <f ca="1">BE5+1</f>
-        <v>45068</v>
+        <v>45075</v>
       </c>
       <c r="BG5" s="10">
         <f ca="1">BF5+1</f>
-        <v>45069</v>
+        <v>45076</v>
       </c>
       <c r="BH5" s="10">
         <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>45070</v>
+        <v>45077</v>
       </c>
       <c r="BI5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>45071</v>
+        <v>45078</v>
       </c>
       <c r="BJ5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>45072</v>
+        <v>45079</v>
       </c>
       <c r="BK5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>45073</v>
+        <v>45080</v>
       </c>
       <c r="BL5" s="12">
         <f t="shared" ca="1" si="2"/>
-        <v>45074</v>
+        <v>45081</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2836,7 +2836,7 @@
         <v>61</v>
       </c>
       <c r="D15" s="27">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E15" s="63">
         <v>44997</v>
@@ -4537,6 +4537,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4544,11 +4549,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
   <conditionalFormatting sqref="D7:D39">

</xml_diff>

<commit_message>
made edits to data feature section and updated Gantt Chart
</commit_message>
<xml_diff>
--- a/Medical Al Disease Diagnostic Tool.Gantt.Chart.xlsx
+++ b/Medical Al Disease Diagnostic Tool.Gantt.Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46AF60B2-EE29-4649-B00B-15C435C78577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38773D1B-D370-F646-8E03-029CC9C33CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="760" windowWidth="26700" windowHeight="17440" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -298,7 +298,7 @@
     <t>Kelvin</t>
   </si>
   <si>
-    <t>Feature engineering</t>
+    <t>Mansoor, Korie</t>
   </si>
 </sst>
 </file>
@@ -1001,6 +1001,13 @@
     <xf numFmtId="0" fontId="27" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1013,13 +1020,6 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1586,11 +1586,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL42"/>
+  <dimension ref="A1:BL41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <pane ySplit="6" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1635,118 +1635,118 @@
       <c r="B3" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="87" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="92"/>
-      <c r="E3" s="90">
+      <c r="D3" s="88"/>
+      <c r="E3" s="93">
         <f ca="1">TODAY()</f>
         <v>45025</v>
       </c>
-      <c r="F3" s="90"/>
+      <c r="F3" s="93"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="91" t="s">
+      <c r="C4" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="92"/>
+      <c r="D4" s="88"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="87">
+      <c r="I4" s="90">
         <f ca="1">I5</f>
         <v>45026</v>
       </c>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="89"/>
-      <c r="P4" s="87">
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="91"/>
+      <c r="O4" s="92"/>
+      <c r="P4" s="90">
         <f ca="1">P5</f>
         <v>45033</v>
       </c>
-      <c r="Q4" s="88"/>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="88"/>
-      <c r="V4" s="89"/>
-      <c r="W4" s="87">
+      <c r="Q4" s="91"/>
+      <c r="R4" s="91"/>
+      <c r="S4" s="91"/>
+      <c r="T4" s="91"/>
+      <c r="U4" s="91"/>
+      <c r="V4" s="92"/>
+      <c r="W4" s="90">
         <f ca="1">W5</f>
         <v>45040</v>
       </c>
-      <c r="X4" s="88"/>
-      <c r="Y4" s="88"/>
-      <c r="Z4" s="88"/>
-      <c r="AA4" s="88"/>
-      <c r="AB4" s="88"/>
-      <c r="AC4" s="89"/>
-      <c r="AD4" s="87">
+      <c r="X4" s="91"/>
+      <c r="Y4" s="91"/>
+      <c r="Z4" s="91"/>
+      <c r="AA4" s="91"/>
+      <c r="AB4" s="91"/>
+      <c r="AC4" s="92"/>
+      <c r="AD4" s="90">
         <f ca="1">AD5</f>
         <v>45047</v>
       </c>
-      <c r="AE4" s="88"/>
-      <c r="AF4" s="88"/>
-      <c r="AG4" s="88"/>
-      <c r="AH4" s="88"/>
-      <c r="AI4" s="88"/>
-      <c r="AJ4" s="89"/>
-      <c r="AK4" s="87">
+      <c r="AE4" s="91"/>
+      <c r="AF4" s="91"/>
+      <c r="AG4" s="91"/>
+      <c r="AH4" s="91"/>
+      <c r="AI4" s="91"/>
+      <c r="AJ4" s="92"/>
+      <c r="AK4" s="90">
         <f ca="1">AK5</f>
         <v>45054</v>
       </c>
-      <c r="AL4" s="88"/>
-      <c r="AM4" s="88"/>
-      <c r="AN4" s="88"/>
-      <c r="AO4" s="88"/>
-      <c r="AP4" s="88"/>
-      <c r="AQ4" s="89"/>
-      <c r="AR4" s="87">
+      <c r="AL4" s="91"/>
+      <c r="AM4" s="91"/>
+      <c r="AN4" s="91"/>
+      <c r="AO4" s="91"/>
+      <c r="AP4" s="91"/>
+      <c r="AQ4" s="92"/>
+      <c r="AR4" s="90">
         <f ca="1">AR5</f>
         <v>45061</v>
       </c>
-      <c r="AS4" s="88"/>
-      <c r="AT4" s="88"/>
-      <c r="AU4" s="88"/>
-      <c r="AV4" s="88"/>
-      <c r="AW4" s="88"/>
-      <c r="AX4" s="89"/>
-      <c r="AY4" s="87">
+      <c r="AS4" s="91"/>
+      <c r="AT4" s="91"/>
+      <c r="AU4" s="91"/>
+      <c r="AV4" s="91"/>
+      <c r="AW4" s="91"/>
+      <c r="AX4" s="92"/>
+      <c r="AY4" s="90">
         <f ca="1">AY5</f>
         <v>45068</v>
       </c>
-      <c r="AZ4" s="88"/>
-      <c r="BA4" s="88"/>
-      <c r="BB4" s="88"/>
-      <c r="BC4" s="88"/>
-      <c r="BD4" s="88"/>
-      <c r="BE4" s="89"/>
-      <c r="BF4" s="87">
+      <c r="AZ4" s="91"/>
+      <c r="BA4" s="91"/>
+      <c r="BB4" s="91"/>
+      <c r="BC4" s="91"/>
+      <c r="BD4" s="91"/>
+      <c r="BE4" s="92"/>
+      <c r="BF4" s="90">
         <f ca="1">BF5</f>
         <v>45075</v>
       </c>
-      <c r="BG4" s="88"/>
-      <c r="BH4" s="88"/>
-      <c r="BI4" s="88"/>
-      <c r="BJ4" s="88"/>
-      <c r="BK4" s="88"/>
-      <c r="BL4" s="89"/>
+      <c r="BG4" s="91"/>
+      <c r="BH4" s="91"/>
+      <c r="BI4" s="91"/>
+      <c r="BJ4" s="91"/>
+      <c r="BK4" s="91"/>
+      <c r="BL4" s="92"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="89"/>
       <c r="I5" s="11">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>45026</v>
@@ -3060,9 +3060,11 @@
       <c r="B18" s="80" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="81"/>
+      <c r="C18" s="81" t="s">
+        <v>74</v>
+      </c>
       <c r="D18" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="63">
         <v>45005</v>
@@ -3135,11 +3137,13 @@
     <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="57"/>
       <c r="B19" s="80" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="81"/>
+        <v>68</v>
+      </c>
+      <c r="C19" s="81" t="s">
+        <v>62</v>
+      </c>
       <c r="D19" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="63">
         <v>45010</v>
@@ -3211,20 +3215,18 @@
     </row>
     <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="57"/>
-      <c r="B20" s="80" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="81" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="27">
-        <v>1</v>
-      </c>
-      <c r="E20" s="63">
-        <v>45011</v>
-      </c>
-      <c r="F20" s="63">
-        <v>45017</v>
+      <c r="B20" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="70"/>
+      <c r="D20" s="29">
+        <v>0</v>
+      </c>
+      <c r="E20" s="30">
+        <v>45006</v>
+      </c>
+      <c r="F20" s="31">
+        <v>45032</v>
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
@@ -3287,17 +3289,17 @@
     </row>
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="57"/>
-      <c r="B21" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="70"/>
-      <c r="D21" s="29">
-        <v>0</v>
-      </c>
-      <c r="E21" s="30">
-        <v>45006</v>
-      </c>
-      <c r="F21" s="31">
+      <c r="B21" s="82" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="71"/>
+      <c r="D21" s="32">
+        <v>0.3</v>
+      </c>
+      <c r="E21" s="64">
+        <v>45007</v>
+      </c>
+      <c r="F21" s="64">
         <v>45032</v>
       </c>
       <c r="G21" s="17"/>
@@ -3362,17 +3364,17 @@
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="57"/>
       <c r="B22" s="82" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C22" s="71"/>
       <c r="D22" s="32">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E22" s="64">
-        <v>45007</v>
+        <v>45006</v>
       </c>
       <c r="F22" s="64">
-        <v>45032</v>
+        <v>45018</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="17"/>
@@ -3436,11 +3438,11 @@
     <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="57"/>
       <c r="B23" s="82" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C23" s="71"/>
       <c r="D23" s="32">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="E23" s="64">
         <v>45006</v>
@@ -3510,7 +3512,7 @@
     <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="57"/>
       <c r="B24" s="82" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="C24" s="71"/>
       <c r="D24" s="32">
@@ -3584,11 +3586,11 @@
     <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="57"/>
       <c r="B25" s="82" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="C25" s="71"/>
       <c r="D25" s="32">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E25" s="64">
         <v>45006</v>
@@ -3658,14 +3660,14 @@
     <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="57"/>
       <c r="B26" s="82" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C26" s="71"/>
       <c r="D26" s="32">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E26" s="64">
-        <v>45006</v>
+        <v>45008</v>
       </c>
       <c r="F26" s="64">
         <v>45018</v>
@@ -3734,14 +3736,14 @@
         <v>24</v>
       </c>
       <c r="B27" s="82" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C27" s="71"/>
       <c r="D27" s="32">
         <v>0</v>
       </c>
       <c r="E27" s="64">
-        <v>45008</v>
+        <v>45012</v>
       </c>
       <c r="F27" s="64">
         <v>45018</v>
@@ -3749,7 +3751,7 @@
       <c r="G27" s="17"/>
       <c r="H27" s="17">
         <f t="shared" si="6"/>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I27" s="44"/>
       <c r="J27" s="44"/>
@@ -3811,14 +3813,14 @@
     <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="57"/>
       <c r="B28" s="82" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C28" s="71"/>
       <c r="D28" s="32">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E28" s="64">
-        <v>45012</v>
+        <v>45011</v>
       </c>
       <c r="F28" s="64">
         <v>45018</v>
@@ -3826,7 +3828,7 @@
       <c r="G28" s="17"/>
       <c r="H28" s="17">
         <f t="shared" si="6"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I28" s="44"/>
       <c r="J28" s="44"/>
@@ -3887,18 +3889,16 @@
     </row>
     <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="57"/>
-      <c r="B29" s="82" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="71"/>
-      <c r="D29" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="E29" s="64">
-        <v>45011</v>
-      </c>
-      <c r="F29" s="64">
-        <v>45018</v>
+      <c r="B29" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="72"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="35">
+        <v>45019</v>
+      </c>
+      <c r="F29" s="36">
+        <v>45032</v>
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="17"/>
@@ -3961,16 +3961,20 @@
     </row>
     <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="57"/>
-      <c r="B30" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="72"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="35">
-        <v>45019</v>
-      </c>
-      <c r="F30" s="36">
-        <v>45032</v>
+      <c r="B30" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="73" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="E30" s="65">
+        <v>45020</v>
+      </c>
+      <c r="F30" s="65">
+        <v>45026</v>
       </c>
       <c r="G30" s="17"/>
       <c r="H30" s="17"/>
@@ -4034,13 +4038,11 @@
     <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="57"/>
       <c r="B31" s="83" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" s="73" t="s">
-        <v>73</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C31" s="73"/>
       <c r="D31" s="37">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E31" s="65">
         <v>45020</v>
@@ -4110,17 +4112,17 @@
     <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="57"/>
       <c r="B32" s="83" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C32" s="73"/>
       <c r="D32" s="37">
         <v>0</v>
       </c>
       <c r="E32" s="65">
-        <v>45020</v>
+        <v>45026</v>
       </c>
       <c r="F32" s="65">
-        <v>45026</v>
+        <v>45029</v>
       </c>
       <c r="G32" s="17"/>
       <c r="H32" s="17"/>
@@ -4184,7 +4186,7 @@
     <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="57"/>
       <c r="B33" s="83" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C33" s="73"/>
       <c r="D33" s="37">
@@ -4258,22 +4260,24 @@
     <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="57"/>
       <c r="B34" s="83" t="s">
-        <v>52</v>
-      </c>
-      <c r="C34" s="73"/>
+        <v>39</v>
+      </c>
+      <c r="C34" s="73" t="s">
+        <v>37</v>
+      </c>
       <c r="D34" s="37">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E34" s="65">
-        <v>45026</v>
+        <v>45029</v>
       </c>
       <c r="F34" s="65">
-        <v>45029</v>
+        <v>45033</v>
       </c>
       <c r="G34" s="17"/>
       <c r="H34" s="17">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I34" s="44"/>
       <c r="J34" s="44"/>
@@ -4337,24 +4341,24 @@
         <v>26</v>
       </c>
       <c r="B35" s="83" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C35" s="73" t="s">
         <v>37</v>
       </c>
       <c r="D35" s="37">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="E35" s="65">
         <v>45029</v>
       </c>
       <c r="F35" s="65">
-        <v>45033</v>
+        <v>45030</v>
       </c>
       <c r="G35" s="17"/>
       <c r="H35" s="17">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I35" s="44"/>
       <c r="J35" s="44"/>
@@ -4418,24 +4422,24 @@
         <v>25</v>
       </c>
       <c r="B36" s="83" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C36" s="73" t="s">
         <v>37</v>
       </c>
       <c r="D36" s="37">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="E36" s="65">
-        <v>45029</v>
+        <v>45047</v>
       </c>
       <c r="F36" s="65">
-        <v>45030</v>
+        <v>45051</v>
       </c>
       <c r="G36" s="43"/>
       <c r="H36" s="43">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I36" s="45"/>
       <c r="J36" s="45"/>
@@ -4495,53 +4499,31 @@
       <c r="BL36" s="45"/>
     </row>
     <row r="37" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="83" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37" s="37">
+      <c r="B37" s="75"/>
+      <c r="C37" s="74"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
+      <c r="G37" s="6"/>
+    </row>
+    <row r="38" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="E37" s="65">
-        <v>45047</v>
-      </c>
-      <c r="F37" s="65">
-        <v>45051</v>
-      </c>
-      <c r="G37" s="6"/>
-    </row>
-    <row r="38" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="75"/>
-      <c r="C38" s="74"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="66"/>
-      <c r="F38" s="66"/>
-    </row>
-    <row r="39" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="39"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="42"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="42"/>
+    </row>
+    <row r="40" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C40" s="14"/>
+      <c r="F40" s="59"/>
     </row>
     <row r="41" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C41" s="14"/>
-      <c r="F41" s="59"/>
-    </row>
-    <row r="42" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C42" s="15"/>
+      <c r="C41" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4549,9 +4531,14 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
-  <conditionalFormatting sqref="D7:D39">
+  <conditionalFormatting sqref="D7:D38">
     <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4605,7 +4592,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D39</xm:sqref>
+          <xm:sqref>D7:D38</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>